<commit_message>
Python imports are going to make me kill someone
</commit_message>
<xml_diff>
--- a/Project notes.xlsx
+++ b/Project notes.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakemoore/Documents/PycharmProjects/CS_493/mooreja2_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120492C7-08FA-454E-807C-47204AAC548C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE107DD-DE08-D443-B263-B64BA9638A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{FFEFC09E-B499-2B42-B339-2866EA5753B9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="4" xr2:uid="{FFEFC09E-B499-2B42-B339-2866EA5753B9}"/>
   </bookViews>
   <sheets>
     <sheet name="All entities " sheetId="1" r:id="rId1"/>
     <sheet name="Data models" sheetId="2" r:id="rId2"/>
     <sheet name="Users" sheetId="3" r:id="rId3"/>
+    <sheet name="methods" sheetId="4" r:id="rId4"/>
+    <sheet name="architecture" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
   <si>
     <t xml:space="preserve">Users </t>
   </si>
@@ -170,16 +172,65 @@
   </si>
   <si>
     <t>Status codes to support:</t>
+  </si>
+  <si>
+    <t>/boats</t>
+  </si>
+  <si>
+    <t>/users</t>
+  </si>
+  <si>
+    <t>/loads</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>/boats/&lt;boat_id&gt;</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>/users/&lt;user_id&gt;</t>
+  </si>
+  <si>
+    <t>/loads/&lt;load_id&gt;</t>
+  </si>
+  <si>
+    <t>models</t>
+  </si>
+  <si>
+    <t>controllers</t>
+  </si>
+  <si>
+    <t>auth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,8 +256,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86398D00-3496-7D4C-A631-DB54C039F342}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
@@ -658,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AF0A95-F016-E947-8CE7-23295C2054E9}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,4 +957,138 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB33107D-A7D5-5448-A84A-CEEA0CDC0A02}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="44.5" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1626D06-ECF4-2B41-9D2C-70FA7731609C}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
weird hangup with put
</commit_message>
<xml_diff>
--- a/Project notes.xlsx
+++ b/Project notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakemoore/Documents/PycharmProjects/CS_493/mooreja2_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE107DD-DE08-D443-B263-B64BA9638A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC08B5-B6B6-A948-80EC-5F5A3F74B611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="4" xr2:uid="{FFEFC09E-B499-2B42-B339-2866EA5753B9}"/>
+    <workbookView xWindow="14320" yWindow="500" windowWidth="30080" windowHeight="21900" activeTab="1" xr2:uid="{FFEFC09E-B499-2B42-B339-2866EA5753B9}"/>
   </bookViews>
   <sheets>
     <sheet name="All entities " sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t xml:space="preserve">Users </t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t xml:space="preserve">Entities should have self attribute </t>
-  </si>
-  <si>
-    <t>last_modified</t>
   </si>
   <si>
     <t xml:space="preserve">Each entity supports CRUD </t>
@@ -622,48 +619,48 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -710,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AF0A95-F016-E947-8CE7-23295C2054E9}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,7 +782,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
@@ -826,28 +823,6 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -931,27 +906,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +939,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,90 +951,84 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
         <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1071,7 +1040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1626D06-ECF4-2B41-9D2C-70FA7731609C}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -1079,13 +1048,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>